<commit_message>
fix menu pos in nav and lang select on login page
</commit_message>
<xml_diff>
--- a/office/translations.xlsx
+++ b/office/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="422">
   <si>
     <t xml:space="preserve">KEY</t>
   </si>
@@ -403,66 +403,10 @@
     <t xml:space="preserve">Die Tageslimite muss im Bereich zwischen {from} und {to} liegen!</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Il limite </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">quotidiano</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> deve essere tra {from} e {to}!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">La limite </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">quotidienne</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> doit être en {from} e {to}!</t>
-    </r>
+    <t xml:space="preserve">Il limite quotidiano deve essere tra {from} e {to}!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La limite quotidienne doit être en {from} e {to}!</t>
   </si>
   <si>
     <t xml:space="preserve">data-protection-header</t>
@@ -1075,6 +1019,21 @@
   </si>
   <si>
     <t xml:space="preserve">Paramètres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">settings-not-stored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings not stored. They will be reverted!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einstellungen nicht gespeichert, werden rückgängig gemacht!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regolazione non salvata, sarà resettata!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les paramètres ne sont pas sauvegardés, ils seront réinitialisés!</t>
   </si>
   <si>
     <t xml:space="preserve">settings-stored-success</t>
@@ -1336,7 +1295,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1367,12 +1326,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1423,7 +1376,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1438,10 +1391,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1529,10 +1478,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2:I91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
@@ -3479,10 +3428,10 @@
       <c r="C60" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E60" s="4" t="s">
         <v>274</v>
       </c>
       <c r="F60" s="1" t="str">
@@ -3916,19 +3865,19 @@
       </c>
       <c r="F73" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A73,""" : """,B73,""",")</f>
-        <v>"settings-stored-success" : "Settings successfully stored!",</v>
+        <v>"settings-not-stored" : "Settings not stored. They will be reverted!",</v>
       </c>
       <c r="G73" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A73,""" : """,C73,""",")</f>
-        <v>"settings-stored-success" : "Die Einstellungen wurden erfolgreich gespeichert!",</v>
+        <v>"settings-not-stored" : "Einstellungen nicht gespeichert, werden rückgängig gemacht!",</v>
       </c>
       <c r="H73" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A73,""" : """,D73,""",")</f>
-        <v>"settings-stored-success" : "La regulazione è stata salvata di successo!",</v>
+        <v>"settings-not-stored" : "Regolazione non salvata, sarà resettata!",</v>
       </c>
       <c r="I73" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A73,""" : """,E73,""",")</f>
-        <v>"settings-stored-success" : "Les paramètres ont étés sauvegardés aves succès!",</v>
+        <v>"settings-not-stored" : "Les paramètres ne sont pas sauvegardés, ils seront réinitialisés!",</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,89 +3894,89 @@
         <v>341</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="F74" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A74,""" : """,B74,""",")</f>
-        <v>"show-confirmations" : "Confirmations",</v>
+        <v>"settings-stored-success" : "Settings successfully stored!",</v>
       </c>
       <c r="G74" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A74,""" : """,C74,""",")</f>
-        <v>"show-confirmations" : "Bestätigungsmeldungen",</v>
+        <v>"settings-stored-success" : "Die Einstellungen wurden erfolgreich gespeichert!",</v>
       </c>
       <c r="H74" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A74,""" : """,D74,""",")</f>
-        <v>"show-confirmations" : "Confirmazioni",</v>
+        <v>"settings-stored-success" : "La regulazione è stata salvata di successo!",</v>
       </c>
       <c r="I74" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A74,""" : """,E74,""",")</f>
-        <v>"show-confirmations" : "Confirmations",</v>
+        <v>"settings-stored-success" : "Les paramètres ont étés sauvegardés aves succès!",</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="F75" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A75,""" : """,B75,""",")</f>
-        <v>"show-notifications" : "Notifications",</v>
+        <v>"show-confirmations" : "Confirmations",</v>
       </c>
       <c r="G75" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A75,""" : """,C75,""",")</f>
-        <v>"show-notifications" : "Notifizierungen",</v>
+        <v>"show-confirmations" : "Bestätigungsmeldungen",</v>
       </c>
       <c r="H75" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A75,""" : """,D75,""",")</f>
-        <v>"show-notifications" : "Notificazioni",</v>
+        <v>"show-confirmations" : "Confirmazioni",</v>
       </c>
       <c r="I75" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A75,""" : """,E75,""",")</f>
-        <v>"show-notifications" : "Notifications",</v>
+        <v>"show-confirmations" : "Confirmations",</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="F76" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A76,""" : """,B76,""",")</f>
-        <v>"start-the-tour" : "Start the tour…",</v>
+        <v>"show-notifications" : "Notifications",</v>
       </c>
       <c r="G76" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A76,""" : """,C76,""",")</f>
-        <v>"start-the-tour" : "Beginne die Tour…",</v>
+        <v>"show-notifications" : "Notifizierungen",</v>
       </c>
       <c r="H76" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A76,""" : """,D76,""",")</f>
-        <v>"start-the-tour" : "Incomincia il giro…",</v>
+        <v>"show-notifications" : "Notificazioni",</v>
       </c>
       <c r="I76" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A76,""" : """,E76,""",")</f>
-        <v>"start-the-tour" : "Commencez le tour…",</v>
+        <v>"show-notifications" : "Notifications",</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4048,22 +3997,22 @@
       </c>
       <c r="F77" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A77,""" : """,B77,""",")</f>
-        <v>"success" : "Success",</v>
+        <v>"start-the-tour" : "Start the tour…",</v>
       </c>
       <c r="G77" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A77,""" : """,C77,""",")</f>
-        <v>"success" : "Erfolg",</v>
+        <v>"start-the-tour" : "Beginne die Tour…",</v>
       </c>
       <c r="H77" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A77,""" : """,D77,""",")</f>
-        <v>"success" : "Successo",</v>
+        <v>"start-the-tour" : "Incomincia il giro…",</v>
       </c>
       <c r="I77" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A77,""" : """,E77,""",")</f>
-        <v>"success" : "Succès",</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"start-the-tour" : "Commencez le tour…",</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>356</v>
       </c>
@@ -4081,19 +4030,19 @@
       </c>
       <c r="F78" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A78,""" : """,B78,""",")</f>
-        <v>"swipe-through-the-tour-" : "Swipe through the Quick-Tour to get an overview of MX-Banklets' features.",</v>
+        <v>"success" : "Success",</v>
       </c>
       <c r="G78" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A78,""" : """,C78,""",")</f>
-        <v>"swipe-through-the-tour-" : "Wischen Sie durch die Quick-Tour, um einen Überblick über die Features der MX-Banklets zu bekommen. ",</v>
+        <v>"success" : "Erfolg",</v>
       </c>
       <c r="H78" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A78,""" : """,D78,""",")</f>
-        <v>"swipe-through-the-tour-" : "Passa a traverso il Quick-Tour per ottenere uno sguardo d'insieme delle funzioni die MX-Banklets.",</v>
+        <v>"success" : "Successo",</v>
       </c>
       <c r="I78" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A78,""" : """,E78,""",")</f>
-        <v>"swipe-through-the-tour-" : "Passez par le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
+        <v>"success" : "Succès",</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4114,22 +4063,22 @@
       </c>
       <c r="F79" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A79,""" : """,B79,""",")</f>
-        <v>"take-the-tour-" : "Take the Quick-Tour to get an overview of MX-Banklets' features.",</v>
+        <v>"swipe-through-the-tour-" : "Swipe through the Quick-Tour to get an overview of MX-Banklets' features.",</v>
       </c>
       <c r="G79" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A79,""" : """,C79,""",")</f>
-        <v>"take-the-tour-" : "Nehmen Sie die Quick-Tour, um einen ersten Überblick über die Features von MX-Banklets zu erhalten.",</v>
+        <v>"swipe-through-the-tour-" : "Wischen Sie durch die Quick-Tour, um einen Überblick über die Features der MX-Banklets zu bekommen. ",</v>
       </c>
       <c r="H79" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A79,""" : """,D79,""",")</f>
-        <v>"take-the-tour-" : "Prenda il Quick-Tour per ottenere un primo sguardo sulle funzioni die MX-Banklets.",</v>
+        <v>"swipe-through-the-tour-" : "Passa a traverso il Quick-Tour per ottenere uno sguardo d'insieme delle funzioni die MX-Banklets.",</v>
       </c>
       <c r="I79" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A79,""" : """,E79,""",")</f>
-        <v>"take-the-tour-" : "Prenez le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"swipe-through-the-tour-" : "Passez par le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>366</v>
       </c>
@@ -4137,67 +4086,67 @@
         <v>367</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F80" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A80,""" : """,B80,""",")</f>
-        <v>"text" : "Text",</v>
+        <v>"take-the-tour-" : "Take the Quick-Tour to get an overview of MX-Banklets' features.",</v>
       </c>
       <c r="G80" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A80,""" : """,C80,""",")</f>
-        <v>"text" : "Text",</v>
+        <v>"take-the-tour-" : "Nehmen Sie die Quick-Tour, um einen ersten Überblick über die Features von MX-Banklets zu erhalten.",</v>
       </c>
       <c r="H80" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A80,""" : """,D80,""",")</f>
-        <v>"text" : "Denominazione",</v>
+        <v>"take-the-tour-" : "Prenda il Quick-Tour per ottenere un primo sguardo sulle funzioni die MX-Banklets.",</v>
       </c>
       <c r="I80" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A80,""" : """,E80,""",")</f>
-        <v>"text" : "Texte",</v>
+        <v>"take-the-tour-" : "Prenez le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F81" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A81,""" : """,B81,""",")</f>
-        <v>"to" : "to",</v>
+        <v>"text" : "Text",</v>
       </c>
       <c r="G81" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A81,""" : """,C81,""",")</f>
-        <v>"to" : "bis",</v>
+        <v>"text" : "Text",</v>
       </c>
       <c r="H81" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A81,""" : """,D81,""",")</f>
-        <v>"to" : "Al",</v>
+        <v>"text" : "Denominazione",</v>
       </c>
       <c r="I81" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A81,""" : """,E81,""",")</f>
-        <v>"to" : "au",</v>
+        <v>"text" : "Texte",</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>375</v>
@@ -4209,56 +4158,56 @@
         <v>377</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="F82" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A82,""" : """,B82,""",")</f>
-        <v>"type" : "Type",</v>
+        <v>"to" : "to",</v>
       </c>
       <c r="G82" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A82,""" : """,C82,""",")</f>
-        <v>"type" : "Typ",</v>
+        <v>"to" : "bis",</v>
       </c>
       <c r="H82" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A82,""" : """,D82,""",")</f>
-        <v>"type" : "Tipo",</v>
+        <v>"to" : "Al",</v>
       </c>
       <c r="I82" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A82,""" : """,E82,""",")</f>
-        <v>"type" : "Type",</v>
+        <v>"to" : "au",</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="F83" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A83,""" : """,B83,""",")</f>
-        <v>"unlock-card" : "Unlock Card",</v>
+        <v>"type" : "Type",</v>
       </c>
       <c r="G83" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A83,""" : """,C83,""",")</f>
-        <v>"unlock-card" : "Karte entsperren",</v>
+        <v>"type" : "Typ",</v>
       </c>
       <c r="H83" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A83,""" : """,D83,""",")</f>
-        <v>"unlock-card" : "Sbloccare la carta",</v>
+        <v>"type" : "Tipo",</v>
       </c>
       <c r="I83" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A83,""" : """,E83,""",")</f>
-        <v>"unlock-card" : "Débloquer la carte",</v>
+        <v>"type" : "Type",</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4279,19 +4228,19 @@
       </c>
       <c r="F84" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A84,""" : """,B84,""",")</f>
-        <v>"username" : "Username",</v>
+        <v>"unlock-card" : "Unlock Card",</v>
       </c>
       <c r="G84" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A84,""" : """,C84,""",")</f>
-        <v>"username" : "Benutzername",</v>
+        <v>"unlock-card" : "Karte entsperren",</v>
       </c>
       <c r="H84" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A84,""" : """,D84,""",")</f>
-        <v>"username" : "Nome utente",</v>
+        <v>"unlock-card" : "Sbloccare la carta",</v>
       </c>
       <c r="I84" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A84,""" : """,E84,""",")</f>
-        <v>"username" : "Nom d'utilisateur",</v>
+        <v>"unlock-card" : "Débloquer la carte",</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4307,24 +4256,24 @@
       <c r="D85" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E85" s="1" t="s">
         <v>392</v>
       </c>
       <c r="F85" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A85,""" : """,B85,""",")</f>
-        <v>"valid-from" : "Valid From",</v>
+        <v>"username" : "Username",</v>
       </c>
       <c r="G85" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A85,""" : """,C85,""",")</f>
-        <v>"valid-from" : "Gültig von",</v>
+        <v>"username" : "Benutzername",</v>
       </c>
       <c r="H85" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A85,""" : """,D85,""",")</f>
-        <v>"valid-from" : "Valido dal",</v>
+        <v>"username" : "Nome utente",</v>
       </c>
       <c r="I85" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A85,""" : """,E85,""",")</f>
-        <v>"valid-from" : "Valable du",</v>
+        <v>"username" : "Nom d'utilisateur",</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4345,19 +4294,19 @@
       </c>
       <c r="F86" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A86,""" : """,B86,""",")</f>
-        <v>"valid-from-to" : "Valid from...to",</v>
+        <v>"valid-from" : "Valid From",</v>
       </c>
       <c r="G86" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A86,""" : """,C86,""",")</f>
-        <v>"valid-from-to" : "Gültig von...bis",</v>
+        <v>"valid-from" : "Gültig von",</v>
       </c>
       <c r="H86" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A86,""" : """,D86,""",")</f>
-        <v>"valid-from-to" : "Valido dal...al",</v>
+        <v>"valid-from" : "Valido dal",</v>
       </c>
       <c r="I86" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A86,""" : """,E86,""",")</f>
-        <v>"valid-from-to" : "Valable du...au",</v>
+        <v>"valid-from" : "Valable du",</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4368,62 +4317,62 @@
         <v>399</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>402</v>
       </c>
       <c r="F87" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A87,""" : """,B87,""",")</f>
-        <v>"version" : "Version",</v>
+        <v>"valid-from-to" : "Valid from...to",</v>
       </c>
       <c r="G87" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A87,""" : """,C87,""",")</f>
-        <v>"version" : "Version",</v>
+        <v>"valid-from-to" : "Gültig von...bis",</v>
       </c>
       <c r="H87" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A87,""" : """,D87,""",")</f>
-        <v>"version" : "Versione",</v>
+        <v>"valid-from-to" : "Valido dal...al",</v>
       </c>
       <c r="I87" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A87,""" : """,E87,""",")</f>
-        <v>"version" : "Version",</v>
+        <v>"valid-from-to" : "Valable du...au",</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>405</v>
       </c>
       <c r="F88" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A88,""" : """,B88,""",")</f>
-        <v>"warning" : "Warning",</v>
+        <v>"version" : "Version",</v>
       </c>
       <c r="G88" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A88,""" : """,C88,""",")</f>
-        <v>"warning" : "Achtung",</v>
+        <v>"version" : "Version",</v>
       </c>
       <c r="H88" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A88,""" : """,D88,""",")</f>
-        <v>"warning" : "Attenzione",</v>
+        <v>"version" : "Versione",</v>
       </c>
       <c r="I88" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A88,""" : """,E88,""",")</f>
-        <v>"warning" : "Attention",</v>
+        <v>"version" : "Version",</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4444,19 +4393,19 @@
       </c>
       <c r="F89" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A89,""" : """,B89,""",")</f>
-        <v>"what-do-you-want-to-do" : "What would you like to do?",</v>
+        <v>"warning" : "Warning",</v>
       </c>
       <c r="G89" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A89,""" : """,C89,""",")</f>
-        <v>"what-do-you-want-to-do" : "Was möchten Sie tun?",</v>
+        <v>"warning" : "Achtung",</v>
       </c>
       <c r="H89" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A89,""" : """,D89,""",")</f>
-        <v>"what-do-you-want-to-do" : "Cosa vuole fare?",</v>
+        <v>"warning" : "Attenzione",</v>
       </c>
       <c r="I89" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A89,""" : """,E89,""",")</f>
-        <v>"what-do-you-want-to-do" : "Qu'est-ce que vous voulez faire?",</v>
+        <v>"warning" : "Attention",</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4477,36 +4426,69 @@
       </c>
       <c r="F90" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A90,""" : """,B90,""",")</f>
-        <v>"yes" : "Yes",</v>
+        <v>"what-do-you-want-to-do" : "What would you like to do?",</v>
       </c>
       <c r="G90" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A90,""" : """,C90,""",")</f>
-        <v>"yes" : "Ja",</v>
+        <v>"what-do-you-want-to-do" : "Was möchten Sie tun?",</v>
       </c>
       <c r="H90" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A90,""" : """,D90,""",")</f>
-        <v>"yes" : "Sì",</v>
+        <v>"what-do-you-want-to-do" : "Cosa vuole fare?",</v>
       </c>
       <c r="I90" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A90,""" : """,E90,""",")</f>
+        <v>"what-do-you-want-to-do" : "Qu'est-ce que vous voulez faire?",</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F91" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A91,""" : """,B91,""",")</f>
+        <v>"yes" : "Yes",</v>
+      </c>
+      <c r="G91" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A91,""" : """,C91,""",")</f>
+        <v>"yes" : "Ja",</v>
+      </c>
+      <c r="H91" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A91,""" : """,D91,""",")</f>
+        <v>"yes" : "Sì",</v>
+      </c>
+      <c r="I91" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A91,""" : """,E91,""",")</f>
         <v>"yes" : "Oui",</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F91" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="92" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F92" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="93" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>